<commit_message>
Avance actualizado de CSS gg
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Quinto Semestre\Programacion web\Curso-full-stack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8221B58F-9FF6-47C1-852C-977F3A13ECF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6168A499-9C90-4892-807B-861CFA51F3A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4215" yWindow="1125" windowWidth="17550" windowHeight="14475" xr2:uid="{277F7D05-DB40-422D-A93B-84EED8012C36}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Bitácora de progreso</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t xml:space="preserve"> 8 -16</t>
+  </si>
+  <si>
+    <t>style.css</t>
   </si>
 </sst>
 </file>
@@ -470,7 +473,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +547,7 @@
       <c r="A7" s="9"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D7" s="10"/>
     </row>

</xml_diff>